<commit_message>
fill missing value with default T
</commit_message>
<xml_diff>
--- a/tests/test_int.xlsx
+++ b/tests/test_int.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\QQPCmgr\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42796466-87C4-4B20-8347-B95333DE8750}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89861A1F-D83E-4FF9-AFDC-3B9B53A6B9C9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -347,7 +347,7 @@
   <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8:F9"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -373,9 +373,6 @@
       <c r="B2">
         <v>7</v>
       </c>
-      <c r="C2">
-        <v>1</v>
-      </c>
       <c r="D2">
         <v>3</v>
       </c>

</xml_diff>